<commit_message>
Latest update and cleanup
</commit_message>
<xml_diff>
--- a/build/output/StructureDefinition-device-patient-used.xlsx
+++ b/build/output/StructureDefinition-device-patient-used.xlsx
@@ -206,7 +206,7 @@
     <t>The definition may point directly to a computable or human-readable definition of the extensibility codes, or it may be a logical URI as declared in some other specification. The definition SHALL be a URI for the Structure Definition defining the extension.</t>
   </si>
   <si>
-    <t>http://pacioproject.org/StructureDefinition/device-patient-used</t>
+    <t>https://paciowg.github.io/cognitive-status-ig/StructureDefinition/device-patient-used</t>
   </si>
   <si>
     <t>N/A</t>
@@ -215,7 +215,7 @@
     <t>Extension.value[x]</t>
   </si>
   <si>
-    <t xml:space="preserve">Reference(http://pacioproject.org/StructureDefinition/pacio-cs-dev)
+    <t xml:space="preserve">Reference(https://paciowg.github.io/cognitive-status-ig/StructureDefinition/pacio-cs-dev)
 </t>
   </si>
   <si>

</xml_diff>

<commit_message>
Use new template hl7.fhir.template and fix QA errors
</commit_message>
<xml_diff>
--- a/build/output/StructureDefinition-device-patient-used.xlsx
+++ b/build/output/StructureDefinition-device-patient-used.xlsx
@@ -206,7 +206,7 @@
     <t>The definition may point directly to a computable or human-readable definition of the extensibility codes, or it may be a logical URI as declared in some other specification. The definition SHALL be a URI for the Structure Definition defining the extension.</t>
   </si>
   <si>
-    <t>https://paciowg.github.io/cognitive-status-ig/StructureDefinition/device-patient-used</t>
+    <t>http://hl7.org/fhir/us/pacio-cs/StructureDefinition/device-patient-used</t>
   </si>
   <si>
     <t>N/A</t>
@@ -215,7 +215,7 @@
     <t>Extension.value[x]</t>
   </si>
   <si>
-    <t xml:space="preserve">Reference(https://paciowg.github.io/cognitive-status-ig/StructureDefinition/pacio-cs-dev)
+    <t xml:space="preserve">Reference(http://hl7.org/fhir/us/pacio-cs/StructureDefinition/pacio-cs-dev)
 </t>
   </si>
   <si>

</xml_diff>

<commit_message>
Remove USCore Observation Lab profile and update instances
</commit_message>
<xml_diff>
--- a/build/output/StructureDefinition-device-patient-used.xlsx
+++ b/build/output/StructureDefinition-device-patient-used.xlsx
@@ -206,7 +206,7 @@
     <t>The definition may point directly to a computable or human-readable definition of the extensibility codes, or it may be a logical URI as declared in some other specification. The definition SHALL be a URI for the Structure Definition defining the extension.</t>
   </si>
   <si>
-    <t>http://hl7.org/fhir/us/pacio-cs/StructureDefinition/device-patient-used</t>
+    <t>http://paciowg.github.io/cognitive-status-ig/StructureDefinition/device-patient-used</t>
   </si>
   <si>
     <t>N/A</t>
@@ -215,7 +215,7 @@
     <t>Extension.value[x]</t>
   </si>
   <si>
-    <t xml:space="preserve">Reference(http://hl7.org/fhir/us/pacio-cs/StructureDefinition/pacio-cs-dev)
+    <t xml:space="preserve">Reference(http://paciowg.github.io/cognitive-status-ig/StructureDefinition/pacio-cs-dev)
 </t>
   </si>
   <si>

</xml_diff>

<commit_message>
Add changes to address ballot comments
</commit_message>
<xml_diff>
--- a/build/output/StructureDefinition-device-patient-used.xlsx
+++ b/build/output/StructureDefinition-device-patient-used.xlsx
@@ -219,7 +219,7 @@
 </t>
   </si>
   <si>
-    <t>Value of extension</t>
+    <t>Points to a record of a healthcare-related assistive device being used by a patient during an assessment.</t>
   </si>
   <si>
     <t>Value of extension - must be one of a constrained set of the data types (see [Extensibility](http://hl7.org/fhir/R4/extensibility.html) for a list).</t>
@@ -394,7 +394,7 @@
     <col min="8" max="8" width="13.2578125" customWidth="true" bestFit="true"/>
     <col min="9" max="9" width="14.44140625" customWidth="true" bestFit="true"/>
     <col min="10" max="10" width="20.703125" customWidth="true" bestFit="true"/>
-    <col min="11" max="11" width="37.171875" customWidth="true" bestFit="true"/>
+    <col min="11" max="11" width="97.76953125" customWidth="true" bestFit="true"/>
     <col min="12" max="12" width="100.703125" customWidth="true" bestFit="true"/>
     <col min="13" max="13" width="100.703125" customWidth="true" bestFit="true"/>
     <col min="14" max="14" width="100.703125" customWidth="true" bestFit="true"/>

</xml_diff>